<commit_message>
Ditambahkan fungsi dan menghapus baris kode yang tidak terpakai
</commit_message>
<xml_diff>
--- a/OutputValidasi.xlsx
+++ b/OutputValidasi.xlsx
@@ -415,10 +415,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>0.8775000000000001</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -451,7 +451,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -462,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -715,7 +715,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -748,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -770,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1089,7 +1089,7 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1199,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1276,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1309,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1518,7 +1518,7 @@
         <v>5</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1661,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1683,7 +1683,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1694,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1705,7 +1705,7 @@
         <v>5</v>
       </c>
       <c r="C119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1892,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1925,7 +1925,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2035,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2178,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2255,7 +2255,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2343,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2365,7 +2365,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2453,7 +2453,7 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2486,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2541,7 +2541,7 @@
         <v>8</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2552,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="C196">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -2695,7 +2695,7 @@
         <v>7</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -2838,7 +2838,7 @@
         <v>8</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -2860,7 +2860,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -2981,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3091,7 +3091,7 @@
         <v>8</v>
       </c>
       <c r="C245">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3113,7 +3113,7 @@
         <v>8</v>
       </c>
       <c r="C247">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3168,7 +3168,7 @@
         <v>5</v>
       </c>
       <c r="C252">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3212,7 +3212,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -3223,7 +3223,7 @@
         <v>7</v>
       </c>
       <c r="C257">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -3289,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -3300,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -3388,7 +3388,7 @@
         <v>5</v>
       </c>
       <c r="C272">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -3410,7 +3410,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -3421,7 +3421,7 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -3454,7 +3454,7 @@
         <v>2</v>
       </c>
       <c r="C278">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -3498,7 +3498,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -3745,10 +3745,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>0.865</v>
+        <v>0.8283333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3781,7 +3781,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3792,7 +3792,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3902,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3990,7 +3990,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4045,7 +4045,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4078,7 +4078,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4100,7 +4100,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4419,7 +4419,7 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -4430,7 +4430,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -4529,7 +4529,7 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -4606,7 +4606,7 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -4639,7 +4639,7 @@
         <v>8</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -4782,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -4848,7 +4848,7 @@
         <v>5</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -4991,7 +4991,7 @@
         <v>2</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -5013,7 +5013,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -5024,7 +5024,7 @@
         <v>8</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -5035,7 +5035,7 @@
         <v>5</v>
       </c>
       <c r="C119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -5222,7 +5222,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -5255,7 +5255,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -5365,7 +5365,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -5508,7 +5508,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -5585,7 +5585,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -5673,7 +5673,7 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -5695,7 +5695,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -5783,7 +5783,7 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -5816,7 +5816,7 @@
         <v>2</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -5871,7 +5871,7 @@
         <v>8</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -5882,7 +5882,7 @@
         <v>5</v>
       </c>
       <c r="C196">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -6025,7 +6025,7 @@
         <v>7</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -6168,7 +6168,7 @@
         <v>8</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -6190,7 +6190,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -6311,7 +6311,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -6421,7 +6421,7 @@
         <v>8</v>
       </c>
       <c r="C245">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -6443,7 +6443,7 @@
         <v>8</v>
       </c>
       <c r="C247">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -6498,7 +6498,7 @@
         <v>5</v>
       </c>
       <c r="C252">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -6542,7 +6542,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -6553,7 +6553,7 @@
         <v>7</v>
       </c>
       <c r="C257">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -6619,7 +6619,7 @@
         <v>2</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -6630,7 +6630,7 @@
         <v>4</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -6718,7 +6718,7 @@
         <v>5</v>
       </c>
       <c r="C272">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -6740,7 +6740,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -6751,7 +6751,7 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -6784,7 +6784,7 @@
         <v>2</v>
       </c>
       <c r="C278">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -6828,7 +6828,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -7075,10 +7075,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>0.86</v>
+        <v>0.8433333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7111,7 +7111,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -7122,7 +7122,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -7232,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -7320,7 +7320,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -7375,7 +7375,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -7408,7 +7408,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -7430,7 +7430,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -7749,7 +7749,7 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -7760,7 +7760,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -7859,7 +7859,7 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -7936,7 +7936,7 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -7969,7 +7969,7 @@
         <v>8</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -8112,7 +8112,7 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -8178,7 +8178,7 @@
         <v>5</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -8321,7 +8321,7 @@
         <v>2</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -8343,7 +8343,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -8354,7 +8354,7 @@
         <v>8</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -8365,7 +8365,7 @@
         <v>5</v>
       </c>
       <c r="C119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -8552,7 +8552,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -8585,7 +8585,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -8695,7 +8695,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -8838,7 +8838,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -8915,7 +8915,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -9003,7 +9003,7 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -9025,7 +9025,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -9113,7 +9113,7 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -9146,7 +9146,7 @@
         <v>2</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -9201,7 +9201,7 @@
         <v>8</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -9212,7 +9212,7 @@
         <v>5</v>
       </c>
       <c r="C196">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -9355,7 +9355,7 @@
         <v>7</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -9498,7 +9498,7 @@
         <v>8</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -9520,7 +9520,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -9641,7 +9641,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -9751,7 +9751,7 @@
         <v>8</v>
       </c>
       <c r="C245">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -9773,7 +9773,7 @@
         <v>8</v>
       </c>
       <c r="C247">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -9828,7 +9828,7 @@
         <v>5</v>
       </c>
       <c r="C252">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -9872,7 +9872,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -9883,7 +9883,7 @@
         <v>7</v>
       </c>
       <c r="C257">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -9949,7 +9949,7 @@
         <v>2</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -9960,7 +9960,7 @@
         <v>4</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -10048,7 +10048,7 @@
         <v>5</v>
       </c>
       <c r="C272">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -10070,7 +10070,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -10081,7 +10081,7 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -10114,7 +10114,7 @@
         <v>2</v>
       </c>
       <c r="C278">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -10158,7 +10158,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -10405,10 +10405,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>0.8558333333333333</v>
+        <v>0.8433333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -10441,7 +10441,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -10452,7 +10452,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -10562,7 +10562,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -10650,7 +10650,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -10705,7 +10705,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -10738,7 +10738,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -10760,7 +10760,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -11079,7 +11079,7 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -11090,7 +11090,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -11189,7 +11189,7 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -11266,7 +11266,7 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -11299,7 +11299,7 @@
         <v>8</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -11442,7 +11442,7 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -11508,7 +11508,7 @@
         <v>5</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -11651,7 +11651,7 @@
         <v>2</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -11673,7 +11673,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -11684,7 +11684,7 @@
         <v>8</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -11695,7 +11695,7 @@
         <v>5</v>
       </c>
       <c r="C119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -11882,7 +11882,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -11915,7 +11915,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -12025,7 +12025,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -12168,7 +12168,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -12245,7 +12245,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -12333,7 +12333,7 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -12355,7 +12355,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -12443,7 +12443,7 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -12476,7 +12476,7 @@
         <v>2</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -12531,7 +12531,7 @@
         <v>8</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -12542,7 +12542,7 @@
         <v>5</v>
       </c>
       <c r="C196">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -12685,7 +12685,7 @@
         <v>7</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -12828,7 +12828,7 @@
         <v>8</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -12850,7 +12850,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -12971,7 +12971,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -13081,7 +13081,7 @@
         <v>8</v>
       </c>
       <c r="C245">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -13103,7 +13103,7 @@
         <v>8</v>
       </c>
       <c r="C247">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -13158,7 +13158,7 @@
         <v>5</v>
       </c>
       <c r="C252">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -13202,7 +13202,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -13213,7 +13213,7 @@
         <v>7</v>
       </c>
       <c r="C257">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -13279,7 +13279,7 @@
         <v>2</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -13290,7 +13290,7 @@
         <v>4</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -13378,7 +13378,7 @@
         <v>5</v>
       </c>
       <c r="C272">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -13400,7 +13400,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -13411,7 +13411,7 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -13444,7 +13444,7 @@
         <v>2</v>
       </c>
       <c r="C278">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -13488,7 +13488,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:3">
@@ -13735,10 +13735,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>0.8416666666666668</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -13771,7 +13771,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -13782,7 +13782,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -13892,7 +13892,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -13980,7 +13980,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -14035,7 +14035,7 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -14068,7 +14068,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -14090,7 +14090,7 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -14409,7 +14409,7 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -14420,7 +14420,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -14519,7 +14519,7 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -14596,7 +14596,7 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -14629,7 +14629,7 @@
         <v>8</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -14772,7 +14772,7 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -14838,7 +14838,7 @@
         <v>5</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -14981,7 +14981,7 @@
         <v>2</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -15003,7 +15003,7 @@
         <v>3</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -15014,7 +15014,7 @@
         <v>8</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -15025,7 +15025,7 @@
         <v>5</v>
       </c>
       <c r="C119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -15212,7 +15212,7 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -15245,7 +15245,7 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -15355,7 +15355,7 @@
         <v>2</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -15498,7 +15498,7 @@
         <v>3</v>
       </c>
       <c r="C162">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -15575,7 +15575,7 @@
         <v>2</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -15663,7 +15663,7 @@
         <v>2</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -15685,7 +15685,7 @@
         <v>3</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -15773,7 +15773,7 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -15806,7 +15806,7 @@
         <v>2</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -15861,7 +15861,7 @@
         <v>8</v>
       </c>
       <c r="C195">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -15872,7 +15872,7 @@
         <v>5</v>
       </c>
       <c r="C196">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -16015,7 +16015,7 @@
         <v>7</v>
       </c>
       <c r="C209">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -16158,7 +16158,7 @@
         <v>8</v>
       </c>
       <c r="C222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -16180,7 +16180,7 @@
         <v>3</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -16301,7 +16301,7 @@
         <v>3</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -16411,7 +16411,7 @@
         <v>8</v>
       </c>
       <c r="C245">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -16433,7 +16433,7 @@
         <v>8</v>
       </c>
       <c r="C247">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -16488,7 +16488,7 @@
         <v>5</v>
       </c>
       <c r="C252">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -16532,7 +16532,7 @@
         <v>6</v>
       </c>
       <c r="C256">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -16543,7 +16543,7 @@
         <v>7</v>
       </c>
       <c r="C257">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -16609,7 +16609,7 @@
         <v>2</v>
       </c>
       <c r="C263">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -16620,7 +16620,7 @@
         <v>4</v>
       </c>
       <c r="C264">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -16708,7 +16708,7 @@
         <v>5</v>
       </c>
       <c r="C272">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:3">
@@ -16730,7 +16730,7 @@
         <v>6</v>
       </c>
       <c r="C274">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -16741,7 +16741,7 @@
         <v>7</v>
       </c>
       <c r="C275">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -16774,7 +16774,7 @@
         <v>2</v>
       </c>
       <c r="C278">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -16818,7 +16818,7 @@
         <v>3</v>
       </c>
       <c r="C282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:3">

</xml_diff>